<commit_message>
bug fixes webappdata take out fuel taxes policy and bcpuc fix #na error
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BCpUC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Mexico\eps-mexico\InputData\elec\BCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C6F2EA-4A60-4C7E-ADE8-36917C57C687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FB32BC-7C2C-4D6E-8005-A7950567DD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -634,7 +634,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -642,51 +642,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -719,27 +715,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2325,26 +2310,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.1796875" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2352,215 +2337,204 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2014</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>2013</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>2021</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="8" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="8" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
-    </row>
-    <row r="46" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="8">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>1.0549999999999999</v>
       </c>
       <c r="B48" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="43">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="38">
         <v>0.9143273584567535</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2582,17 +2556,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="33.36328125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>2019</v>
       </c>
@@ -2690,7 +2664,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -2797,7 +2771,7 @@
         <v>205.4624</v>
       </c>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>73</v>
       </c>
@@ -2898,7 +2872,7 @@
         <v>384.774771419959</v>
       </c>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>74</v>
       </c>
@@ -2999,7 +2973,7 @@
         <v>594.1617</v>
       </c>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>75</v>
       </c>
@@ -3100,7 +3074,7 @@
         <v>345.73</v>
       </c>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>76</v>
       </c>
@@ -3201,7 +3175,7 @@
         <v>588.07036627634386</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>77</v>
       </c>
@@ -3302,7 +3276,7 @@
         <v>980.8854</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>78</v>
       </c>
@@ -3403,7 +3377,7 @@
         <v>485.99760000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>79</v>
       </c>
@@ -3504,7 +3478,7 @@
         <v>791.36596113272867</v>
       </c>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>80</v>
       </c>
@@ -3605,7 +3579,7 @@
         <v>1367.6091000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>81</v>
       </c>
@@ -3706,7 +3680,7 @@
         <v>626.26520000000005</v>
       </c>
     </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>82</v>
       </c>
@@ -3807,7 +3781,7 @@
         <v>994.66155598911359</v>
       </c>
     </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>83</v>
       </c>
@@ -3908,7 +3882,7 @@
         <v>1754.3328000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>84</v>
       </c>
@@ -4009,7 +3983,7 @@
         <v>766.53280000000007</v>
       </c>
     </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>85</v>
       </c>
@@ -4110,7 +4084,7 @@
         <v>1197.9571508454985</v>
       </c>
     </row>
-    <row r="17" spans="5:37" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:37" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>86</v>
       </c>
@@ -4224,776 +4198,775 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" style="10" customWidth="1"/>
-    <col min="2" max="13" width="11.26953125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="10"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="13" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="19"/>
-      <c r="B2" s="46" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="49" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="49" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="50"/>
-      <c r="M2" s="51"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="L2" s="41"/>
+      <c r="M2" s="42"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="9">
         <v>50160000</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="12">
         <v>209</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <v>0.84</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="13">
         <v>25080000</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="12">
         <v>209</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="10">
         <v>0.42</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="13">
         <v>12540000</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="12">
         <v>209</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="10">
         <v>0.21</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="13">
         <v>6270000</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="12">
         <v>209</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="10">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="9">
         <v>4200000</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="12">
         <v>18</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="13">
         <v>4200000</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="12">
         <v>35</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="13">
         <v>4200000</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="12">
         <v>70</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="13">
         <v>4200000</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="12">
         <v>140</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="9">
         <v>3121131</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <v>13</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="10">
         <v>0.05</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="13">
         <v>1813452</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="12">
         <v>15</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="10">
         <v>0.03</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="13">
         <v>1159612</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="12">
         <v>19</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="10">
         <v>0.02</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="13">
         <v>832692</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="12">
         <v>28</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="9">
         <v>8602825</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>36</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="13">
         <v>6119167</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>51</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="10">
         <v>0.1</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="13">
         <v>4877337</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="12">
         <v>81</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="10">
         <v>0.08</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="13">
         <v>4256423</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="12">
         <v>142</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="9">
         <v>5479149</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="12">
         <v>23</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="10">
         <v>0.09</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="13">
         <v>4322275</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="12">
         <v>36</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="13">
         <v>3743838</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="12">
         <v>62</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="10">
         <v>0.06</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="13">
         <v>3454619</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="12">
         <v>115</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="10">
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="9">
         <v>2775545</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>12</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="10">
         <v>0.05</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="13">
         <v>1948565</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>16</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="10">
         <v>0.03</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="13">
         <v>1535075</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="12">
         <v>26</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="10">
         <v>0.03</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="13">
         <v>1328330</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="12">
         <v>44</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="10">
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="9">
         <v>5293460</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="12">
         <v>22</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="10">
         <v>0.09</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="13">
         <v>3083292</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="12">
         <v>26</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="10">
         <v>0.05</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="13">
         <v>1978209</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="12">
         <v>33</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="10">
         <v>0.03</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="13">
         <v>1425667</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="12">
         <v>48</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="10">
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="23">
         <v>79632110</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="24">
         <v>332</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="25">
         <v>1.33</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="26">
         <v>46566751</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="24">
         <v>388</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="25">
         <v>0.78</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="26">
         <v>30034071</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="24">
         <v>501</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="25">
         <v>0.5</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="26">
         <v>21767732</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="24">
         <v>726</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="25">
         <v>0.36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="7">
         <v>250000</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <v>0</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <v>250000</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="8">
         <v>2</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="11">
         <v>0</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>250000</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="8">
         <v>4</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="11">
         <v>0</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="14">
         <v>250000</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="8">
         <v>8</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="9">
         <v>295289</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="12">
         <v>1</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="10">
         <v>0</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="13">
         <v>295289</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="12">
         <v>2</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="10">
         <v>0</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="13">
         <v>295289</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="12">
         <v>5</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="10">
         <v>0</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="13">
         <v>295289</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="12">
         <v>10</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="9">
         <v>1802363</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="12">
         <v>8</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="10">
         <v>0.03</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="13">
         <v>1802363</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="12">
         <v>15</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="10">
         <v>0.03</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="13">
         <v>1802363</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="12">
         <v>30</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="10">
         <v>0.03</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="13">
         <v>1802363</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="12">
         <v>60</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="10">
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="9">
         <v>2477135</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="12">
         <v>10</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="10">
         <v>0.04</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="13">
         <v>1476303</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="12">
         <v>12</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="10">
         <v>0.02</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="13">
         <v>975887</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="12">
         <v>16</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="10">
         <v>0.02</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="13">
         <v>725679</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="12">
         <v>24</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="9">
         <v>2477135</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="12">
         <v>10</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="10">
         <v>0.04</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="13">
         <v>1476303</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="12">
         <v>12</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="10">
         <v>0.02</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="13">
         <v>975887</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="12">
         <v>16</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="10">
         <v>0.02</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="13">
         <v>725679</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="12">
         <v>24</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="9">
         <v>4346702</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <v>18</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="13">
         <v>2593350</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="12">
         <v>22</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="10">
         <v>0.04</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="13">
         <v>1716675</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="12">
         <v>29</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="10">
         <v>0.03</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="13">
         <v>1278337</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="12">
         <v>43</v>
       </c>
-      <c r="M17" s="14">
+      <c r="M17" s="10">
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="28">
         <v>11648623</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="29">
         <v>49</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="30">
         <v>0.19</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="31">
         <v>7893608</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="29">
         <v>66</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="30">
         <v>0.13</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="31">
         <v>6016101</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="29">
         <v>100</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="30">
         <v>0.1</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="31">
         <v>5077347</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="29">
         <v>169</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="30">
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="35">
         <f>SUM(D5:D9,D12:D17)</f>
         <v>0.57999999999999985</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="40" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="36">
         <f>D10*SUM(D5:D7)/SUM(D4:D7)</f>
         <v>2.1272727272727273E-2</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="40" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="35">
         <f>SUM(D22:D23)</f>
         <v>0.60127272727272707</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="40" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="5">
         <f>D24*10^6</f>
         <v>601272.72727272706</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="40" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="44">
+      <c r="D26" s="5">
         <f>D25*About!A49</f>
         <v>549760.10443936056</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>68</v>
       </c>
     </row>
@@ -5017,258 +4990,258 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="8" customWidth="1"/>
-    <col min="3" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="32" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8">
+      <c r="B1">
         <v>2020</v>
       </c>
-      <c r="C1" s="8">
+      <c r="C1">
         <v>2021</v>
       </c>
-      <c r="D1" s="8">
+      <c r="D1">
         <v>2022</v>
       </c>
-      <c r="E1" s="8">
+      <c r="E1">
         <v>2023</v>
       </c>
-      <c r="F1" s="8">
+      <c r="F1">
         <v>2024</v>
       </c>
-      <c r="G1" s="8">
+      <c r="G1">
         <v>2025</v>
       </c>
-      <c r="H1" s="8">
+      <c r="H1">
         <v>2026</v>
       </c>
-      <c r="I1" s="8">
+      <c r="I1">
         <v>2027</v>
       </c>
-      <c r="J1" s="8">
+      <c r="J1">
         <v>2028</v>
       </c>
-      <c r="K1" s="8">
+      <c r="K1">
         <v>2029</v>
       </c>
-      <c r="L1" s="8">
+      <c r="L1">
         <v>2030</v>
       </c>
-      <c r="M1" s="8">
+      <c r="M1">
         <v>2031</v>
       </c>
-      <c r="N1" s="8">
+      <c r="N1">
         <v>2032</v>
       </c>
-      <c r="O1" s="8">
+      <c r="O1">
         <v>2033</v>
       </c>
-      <c r="P1" s="8">
+      <c r="P1">
         <v>2034</v>
       </c>
-      <c r="Q1" s="8">
+      <c r="Q1">
         <v>2035</v>
       </c>
-      <c r="R1" s="8">
+      <c r="R1">
         <v>2036</v>
       </c>
-      <c r="S1" s="8">
+      <c r="S1">
         <v>2037</v>
       </c>
-      <c r="T1" s="8">
+      <c r="T1">
         <v>2038</v>
       </c>
-      <c r="U1" s="8">
+      <c r="U1">
         <v>2039</v>
       </c>
-      <c r="V1" s="8">
+      <c r="V1">
         <v>2040</v>
       </c>
-      <c r="W1" s="8">
+      <c r="W1">
         <v>2041</v>
       </c>
-      <c r="X1" s="8">
+      <c r="X1">
         <v>2042</v>
       </c>
-      <c r="Y1" s="8">
+      <c r="Y1">
         <v>2043</v>
       </c>
-      <c r="Z1" s="8">
+      <c r="Z1">
         <v>2044</v>
       </c>
-      <c r="AA1" s="8">
+      <c r="AA1">
         <v>2045</v>
       </c>
-      <c r="AB1" s="8">
+      <c r="AB1">
         <v>2046</v>
       </c>
-      <c r="AC1" s="8">
+      <c r="AC1">
         <v>2047</v>
       </c>
-      <c r="AD1" s="8">
+      <c r="AD1">
         <v>2048</v>
       </c>
-      <c r="AE1" s="8">
+      <c r="AE1">
         <v>2049</v>
       </c>
-      <c r="AF1" s="8">
+      <c r="AF1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(B1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>1363284.234215365</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(C1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>1281813.0648399449</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(D1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>1200341.8954645249</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(E1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>1118870.7260891048</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(F1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>1037399.5567136847</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(G1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>955928.38733826403</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(H1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>921561.47421096952</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(I1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>887194.56108367513</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(J1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>852827.64795638062</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(K1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>818460.734829086</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(L1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>784093.82170179195</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(M1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>774292.64893051935</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(N1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>764491.47615924687</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(O1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>754690.30338797462</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(P1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>744889.13061670202</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(Q1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>735087.95784542954</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(R1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>725286.78507415717</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(S1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>715485.61230288458</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(T1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>705684.43953161221</v>
       </c>
-      <c r="U2" s="6">
+      <c r="U2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(U1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>695883.26676033961</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(V1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>686082.09398906713</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(W1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>676280.92121779488</v>
       </c>
-      <c r="X2" s="6">
+      <c r="X2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(X1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>666479.74844652251</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Y2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(Y1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>656678.57567524991</v>
       </c>
-      <c r="Z2" s="6">
+      <c r="Z2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(Z1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>646877.40290397755</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="AA2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(AA1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>637076.2301327053</v>
       </c>
-      <c r="AB2" s="6">
+      <c r="AB2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(AB1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>627275.05736143282</v>
       </c>
-      <c r="AC2" s="6">
+      <c r="AC2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(AC1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>617473.88459016045</v>
       </c>
-      <c r="AD2" s="6">
+      <c r="AD2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(AD1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>607672.71181888808</v>
       </c>
-      <c r="AE2" s="6">
+      <c r="AE2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(AE1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>597871.5390476156</v>
       </c>
-      <c r="AF2" s="6">
+      <c r="AF2" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(AF1,'NREL ATB'!$2:$2,0))*1000</f>
         <v>588070.36627634382</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>2020</v>
       </c>
       <c r="C7">
@@ -5362,20 +5335,20 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="39">
         <v>1363280</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="39">
         <v>1220010</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="39">
         <v>1125280</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="39">
         <v>1055380</v>
       </c>
       <c r="F8">
@@ -5460,137 +5433,137 @@
         <v>662505</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f>B2-B8</f>
         <v>4.2342153650242835</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f t="shared" ref="C10:AF10" si="0">C2-C8</f>
         <v>61803.064839944942</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>75061.89546452486</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>63490.726089104777</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>37582.556713684695</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>1151.3873382640304</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
         <v>5815.4742109695217</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <f t="shared" si="0"/>
         <v>5304.5610836751293</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <f t="shared" si="0"/>
         <v>67.647956380620599</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <f t="shared" si="0"/>
         <v>-9298.2651709140046</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <f t="shared" si="0"/>
         <v>-22152.178298208048</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="5">
         <f t="shared" si="0"/>
         <v>-13269.351069480646</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="5">
         <f t="shared" si="0"/>
         <v>-7018.5238407531288</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="5">
         <f t="shared" si="0"/>
         <v>-3072.6966120253783</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="5">
         <f t="shared" si="0"/>
         <v>-976.86938329797704</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="5">
         <f t="shared" si="0"/>
         <v>-333.04215457045939</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="5">
         <f t="shared" si="0"/>
         <v>-966.21492584282532</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="5">
         <f t="shared" si="0"/>
         <v>-2707.3876971154241</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="5">
         <f t="shared" si="0"/>
         <v>-5348.56046838779</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U10" s="5">
         <f t="shared" si="0"/>
         <v>-8711.7332396603888</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="5">
         <f t="shared" si="0"/>
         <v>-12672.906010932871</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="5">
         <f t="shared" si="0"/>
         <v>-17237.078782205121</v>
       </c>
-      <c r="X10" s="6">
+      <c r="X10" s="5">
         <f t="shared" si="0"/>
         <v>-22299.251553477487</v>
       </c>
-      <c r="Y10" s="6">
+      <c r="Y10" s="5">
         <f t="shared" si="0"/>
         <v>-27796.424324750085</v>
       </c>
-      <c r="Z10" s="6">
+      <c r="Z10" s="5">
         <f t="shared" si="0"/>
         <v>-33664.597096022451</v>
       </c>
-      <c r="AA10" s="6">
+      <c r="AA10" s="5">
         <f t="shared" si="0"/>
         <v>-39853.769867294701</v>
       </c>
-      <c r="AB10" s="6">
+      <c r="AB10" s="5">
         <f t="shared" si="0"/>
         <v>-46331.942638567183</v>
       </c>
-      <c r="AC10" s="6">
+      <c r="AC10" s="5">
         <f t="shared" si="0"/>
         <v>-53057.115409839549</v>
       </c>
-      <c r="AD10" s="6">
+      <c r="AD10" s="5">
         <f t="shared" si="0"/>
         <v>-59997.288181111915</v>
       </c>
-      <c r="AE10" s="6">
+      <c r="AE10" s="5">
         <f t="shared" si="0"/>
         <v>-67131.460952384397</v>
       </c>
-      <c r="AF10" s="6">
+      <c r="AF10" s="5">
         <f t="shared" si="0"/>
         <v>-74434.633723656181</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>96</v>
       </c>
     </row>
@@ -5607,310 +5580,310 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
-      <c r="B2" s="6" t="e">
-        <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A2,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A2,BBoSCpUC!$1:$1,0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
+      <c r="B2" s="5">
+        <f>B3</f>
+        <v>813519.89556063944</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2020</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A3,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A3,BBoSCpUC!$1:$1,0))</f>
         <v>813519.89556063944</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2021</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A4,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A4,BBoSCpUC!$1:$1,0))</f>
         <v>670249.89556063944</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2022</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A5,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A5,BBoSCpUC!$1:$1,0))</f>
         <v>575519.89556063944</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2023</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A6,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A6,BBoSCpUC!$1:$1,0))</f>
         <v>505619.89556063944</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2024</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A7,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A7,BBoSCpUC!$1:$1,0))</f>
         <v>450056.89556063944</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2025</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A8,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A8,BBoSCpUC!$1:$1,0))</f>
         <v>405016.89556063944</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>2026</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A9,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A9,BBoSCpUC!$1:$1,0))</f>
         <v>365985.89556063944</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="8">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>2027</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A10,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A10,BBoSCpUC!$1:$1,0))</f>
         <v>332129.89556063944</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="8">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2028</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A11,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A11,BBoSCpUC!$1:$1,0))</f>
         <v>302999.89556063944</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="8">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2029</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A12,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A12,BBoSCpUC!$1:$1,0))</f>
         <v>277998.89556063944</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="8">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2030</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A13,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A13,BBoSCpUC!$1:$1,0))</f>
         <v>256485.89556063944</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>2031</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A14,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A14,BBoSCpUC!$1:$1,0))</f>
         <v>237801.89556063944</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>2032</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A15,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A15,BBoSCpUC!$1:$1,0))</f>
         <v>221749.89556063944</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>2033</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A16,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A16,BBoSCpUC!$1:$1,0))</f>
         <v>208002.89556063944</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>2034</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A17,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A17,BBoSCpUC!$1:$1,0))</f>
         <v>196105.89556063944</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="8">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>2035</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A18,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A18,BBoSCpUC!$1:$1,0))</f>
         <v>185660.89556063944</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="8">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>2036</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A19,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A19,BBoSCpUC!$1:$1,0))</f>
         <v>176492.89556063944</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="8">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>2037</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A20,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A20,BBoSCpUC!$1:$1,0))</f>
         <v>168432.89556063944</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="8">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>2038</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A21,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A21,BBoSCpUC!$1:$1,0))</f>
         <v>161272.89556063944</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="8">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>2039</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A22,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A22,BBoSCpUC!$1:$1,0))</f>
         <v>154834.89556063944</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="8">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>2040</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A23,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A23,BBoSCpUC!$1:$1,0))</f>
         <v>148994.89556063944</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>2041</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A24,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A24,BBoSCpUC!$1:$1,0))</f>
         <v>143757.89556063944</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>2042</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A25,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A25,BBoSCpUC!$1:$1,0))</f>
         <v>139018.89556063944</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>2043</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A26,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A26,BBoSCpUC!$1:$1,0))</f>
         <v>134714.89556063944</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="8">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>2044</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A27,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A27,BBoSCpUC!$1:$1,0))</f>
         <v>130781.89556063944</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="8">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>2045</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A28,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A28,BBoSCpUC!$1:$1,0))</f>
         <v>127169.89556063944</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="8">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>2046</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A29,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A29,BBoSCpUC!$1:$1,0))</f>
         <v>123846.89556063944</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="8">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>2047</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A30,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A30,BBoSCpUC!$1:$1,0))</f>
         <v>120770.89556063944</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="8">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>2048</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A31,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A31,BBoSCpUC!$1:$1,0))</f>
         <v>117909.89556063944</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="8">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>2049</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A32,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A32,BBoSCpUC!$1:$1,0))</f>
         <v>115242.89556063944</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="8">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>2050</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A33,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A33,BBoSCpUC!$1:$1,0))</f>
         <v>112744.89556063944</v>
       </c>
@@ -5931,234 +5904,234 @@
       <selection activeCell="B2" sqref="B2:AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="8">
+      <c r="B1">
         <v>2020</v>
       </c>
-      <c r="C1" s="8">
+      <c r="C1">
         <v>2021</v>
       </c>
-      <c r="D1" s="8">
+      <c r="D1">
         <v>2022</v>
       </c>
-      <c r="E1" s="8">
+      <c r="E1">
         <v>2023</v>
       </c>
-      <c r="F1" s="8">
+      <c r="F1">
         <v>2024</v>
       </c>
-      <c r="G1" s="8">
+      <c r="G1">
         <v>2025</v>
       </c>
-      <c r="H1" s="8">
+      <c r="H1">
         <v>2026</v>
       </c>
-      <c r="I1" s="8">
+      <c r="I1">
         <v>2027</v>
       </c>
-      <c r="J1" s="8">
+      <c r="J1">
         <v>2028</v>
       </c>
-      <c r="K1" s="8">
+      <c r="K1">
         <v>2029</v>
       </c>
-      <c r="L1" s="8">
+      <c r="L1">
         <v>2030</v>
       </c>
-      <c r="M1" s="8">
+      <c r="M1">
         <v>2031</v>
       </c>
-      <c r="N1" s="8">
+      <c r="N1">
         <v>2032</v>
       </c>
-      <c r="O1" s="8">
+      <c r="O1">
         <v>2033</v>
       </c>
-      <c r="P1" s="8">
+      <c r="P1">
         <v>2034</v>
       </c>
-      <c r="Q1" s="8">
+      <c r="Q1">
         <v>2035</v>
       </c>
-      <c r="R1" s="8">
+      <c r="R1">
         <v>2036</v>
       </c>
-      <c r="S1" s="8">
+      <c r="S1">
         <v>2037</v>
       </c>
-      <c r="T1" s="8">
+      <c r="T1">
         <v>2038</v>
       </c>
-      <c r="U1" s="8">
+      <c r="U1">
         <v>2039</v>
       </c>
-      <c r="V1" s="8">
+      <c r="V1">
         <v>2040</v>
       </c>
-      <c r="W1" s="8">
+      <c r="W1">
         <v>2041</v>
       </c>
-      <c r="X1" s="8">
+      <c r="X1">
         <v>2042</v>
       </c>
-      <c r="Y1" s="8">
+      <c r="Y1">
         <v>2043</v>
       </c>
-      <c r="Z1" s="8">
+      <c r="Z1">
         <v>2044</v>
       </c>
-      <c r="AA1" s="8">
+      <c r="AA1">
         <v>2045</v>
       </c>
-      <c r="AB1" s="8">
+      <c r="AB1">
         <v>2046</v>
       </c>
-      <c r="AC1" s="8">
+      <c r="AC1">
         <v>2047</v>
       </c>
-      <c r="AD1" s="8">
+      <c r="AD1">
         <v>2048</v>
       </c>
-      <c r="AE1" s="8">
+      <c r="AE1">
         <v>2049</v>
       </c>
-      <c r="AF1" s="8">
+      <c r="AF1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!B10</f>
         <v>549764.33865472558</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!C10</f>
         <v>611563.1692793055</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!D10</f>
         <v>624821.99990388541</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!E10</f>
         <v>613250.83052846533</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!F10</f>
         <v>587342.66115304525</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!G10</f>
         <v>550911.49177762459</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!H10</f>
         <v>555575.57865033008</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!I10</f>
         <v>555064.66552303568</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!J10</f>
         <v>549827.75239574118</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!K10</f>
         <v>540461.83926844655</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!L10</f>
         <v>527607.92614115251</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!M10</f>
         <v>536490.75336987991</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!N10</f>
         <v>542741.58059860743</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!O10</f>
         <v>546687.40782733518</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!P10</f>
         <v>548783.23505606258</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!Q10</f>
         <v>549427.0622847901</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!R10</f>
         <v>548793.88951351773</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!S10</f>
         <v>547052.71674224513</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!T10</f>
         <v>544411.54397097277</v>
       </c>
-      <c r="U2" s="6">
+      <c r="U2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!U10</f>
         <v>541048.37119970017</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!V10</f>
         <v>537087.19842842768</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!W10</f>
         <v>532523.02565715543</v>
       </c>
-      <c r="X2" s="6">
+      <c r="X2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!X10</f>
         <v>527460.85288588307</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Y2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!Y10</f>
         <v>521963.68011461047</v>
       </c>
-      <c r="Z2" s="6">
+      <c r="Z2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!Z10</f>
         <v>516095.5073433381</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="AA2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!AA10</f>
         <v>509906.33457206585</v>
       </c>
-      <c r="AB2" s="6">
+      <c r="AB2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!AB10</f>
         <v>503428.16180079337</v>
       </c>
-      <c r="AC2" s="6">
+      <c r="AC2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!AC10</f>
         <v>496702.98902952101</v>
       </c>
-      <c r="AD2" s="6">
+      <c r="AD2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!AD10</f>
         <v>489762.81625824864</v>
       </c>
-      <c r="AE2" s="6">
+      <c r="AE2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!AE10</f>
         <v>482628.64348697616</v>
       </c>
-      <c r="AF2" s="6">
+      <c r="AF2" s="5">
         <f>'Balance of System Calculations'!$D$26+'Calibration Check'!AF10</f>
         <v>475325.47071570437</v>
       </c>

</xml_diff>